<commit_message>
reverting back to host 0 and port 8080
</commit_message>
<xml_diff>
--- a/outputs/challenge_match.xlsx
+++ b/outputs/challenge_match.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>AIR-INK: Air-Pollution to ink</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>BMW Foundation Herbert Quandt</t>
-  </si>
-  <si>
-    <t>Buenos Aires Innovation Park (City of Buenos Aires Government)</t>
   </si>
   <si>
     <t>C L Sandberg &amp; Associates</t>
@@ -590,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AG41"/>
+  <dimension ref="A1:AG40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4636,107 +4633,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:33">
-      <c r="A41" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>1</v>
-      </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-      <c r="L41">
-        <v>1</v>
-      </c>
-      <c r="M41">
-        <v>1</v>
-      </c>
-      <c r="N41">
-        <v>1</v>
-      </c>
-      <c r="O41">
-        <v>1</v>
-      </c>
-      <c r="P41">
-        <v>1</v>
-      </c>
-      <c r="Q41">
-        <v>1</v>
-      </c>
-      <c r="R41">
-        <v>1</v>
-      </c>
-      <c r="S41">
-        <v>1</v>
-      </c>
-      <c r="T41">
-        <v>1</v>
-      </c>
-      <c r="U41">
-        <v>1</v>
-      </c>
-      <c r="V41">
-        <v>1</v>
-      </c>
-      <c r="W41">
-        <v>1</v>
-      </c>
-      <c r="X41">
-        <v>1</v>
-      </c>
-      <c r="Y41">
-        <v>1</v>
-      </c>
-      <c r="Z41">
-        <v>1</v>
-      </c>
-      <c r="AA41">
-        <v>1</v>
-      </c>
-      <c r="AB41">
-        <v>1</v>
-      </c>
-      <c r="AC41">
-        <v>1</v>
-      </c>
-      <c r="AD41">
-        <v>1</v>
-      </c>
-      <c r="AE41">
-        <v>1</v>
-      </c>
-      <c r="AF41">
-        <v>1</v>
-      </c>
-      <c r="AG41">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>